<commit_message>
More firms. First time using it
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\IdeaProjects\contactsK\src\main\resources\baseFiles\excel\RawXL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB81CC94-208B-4196-B57B-336E4DE116DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B510A0D-9A4C-43D4-A75A-713448F11C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{EDD5D14D-B0D8-4A16-98F2-AF3F46E1EA6C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Firm</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -491,45 +494,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="27.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="19" style="5" customWidth="1"/>
+    <col min="1" max="4" width="27.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More firms, create new page base site and firms, created a new class that have all the files CONFIG, created a class that contains the logic to collect the data from the registered lawyers file
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\IdeaProjects\contactsK\src\main\resources\baseFiles\excel\RawXL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B510A0D-9A4C-43D4-A75A-713448F11C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{EDD5D14D-B0D8-4A16-98F2-AF3F46E1EA6C}"/>
+    <workbookView windowWidth="23040" windowHeight="9707"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,53 +27,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Firm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Role</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>Nationality</t>
-  </si>
-  <si>
     <t>Practice Area</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Link</t>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Specialism</t>
+  </si>
+  <si>
+    <t>Title at Firm</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Etienne Kairis</t>
+  </si>
+  <si>
+    <t>e.kairis@liedekerke.com</t>
+  </si>
+  <si>
+    <t>+32 2 551 15 72</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Intellectual Property</t>
+  </si>
+  <si>
+    <t>https://liedekerke.com/en/lawyers/kairis-etienne</t>
+  </si>
+  <si>
+    <t>Karine Frois</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Co-managing Partner</t>
+  </si>
+  <si>
+    <t>Liedekerke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -90,10 +112,186 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Candara"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FFCC1013"/>
+      <name val="helvetica"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF111111"/>
+      <name val="helvetica"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FFCC1013"/>
+      <name val="helvetica"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="helvetica"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.8"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +304,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -117,16 +501,86 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -139,39 +593,323 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -220,7 +958,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -253,26 +991,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -305,23 +1026,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -483,63 +1187,113 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="4" width="27.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19" style="5" customWidth="1"/>
+    <col min="1" max="1" width="27.6666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.8916666666667" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6666666666667" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.775" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.225" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.225" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.8916666666667" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.1083333333333" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19" style="3" customWidth="1"/>
+    <col min="10" max="10" width="26.225" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="21.6" customHeight="1" spans="1:10">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:10">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" ht="30" spans="1:10">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="+32 2 551 15 72" tooltip="https://liedekerke.com/en/lawyers/tel:+3225511572"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More files. Fixes in the log class
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9707"/>
+    <workbookView windowWidth="30240" windowHeight="14460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,131 +26,27 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Practice Area</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>Specialism</t>
-  </si>
-  <si>
-    <t>Title at Firm</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Etienne Kairis</t>
-  </si>
-  <si>
-    <t>e.kairis@liedekerke.com</t>
-  </si>
-  <si>
-    <t>+32 2 551 15 72</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Intellectual Property</t>
-  </si>
-  <si>
-    <t>https://liedekerke.com/en/lawyers/kairis-etienne</t>
-  </si>
-  <si>
-    <t>Karine Frois</t>
-  </si>
-  <si>
-    <t>Legal</t>
-  </si>
-  <si>
-    <t>Co-managing Partner</t>
-  </si>
-  <si>
-    <t>Liedekerke</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Candara"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color rgb="FFCC1013"/>
-      <name val="helvetica"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="13.5"/>
-      <color rgb="FF111111"/>
-      <name val="helvetica"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="13.5"/>
-      <color rgb="FFCC1013"/>
-      <name val="helvetica"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF111111"/>
-      <name val="helvetica"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9.8"/>
-      <color rgb="FF6A8759"/>
-      <name val="Courier New"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -158,14 +54,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -173,7 +69,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -181,7 +77,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -189,7 +85,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -197,7 +93,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -205,14 +101,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -220,7 +116,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -228,7 +124,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -236,14 +132,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -251,47 +147,47 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,12 +196,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -491,82 +381,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -581,15 +401,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,8 +489,10 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -688,172 +501,146 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,7 +649,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -906,7 +693,221 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -916,7 +917,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -926,44 +927,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -993,12 +994,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1087,6 +1088,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1095,13 +1103,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1166,134 +1167,22 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J3"/>
+  <sheetPr/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="2"/>
-  <cols>
-    <col min="1" max="1" width="27.6666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.8916666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.6666666666667" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.775" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.225" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.225" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.8916666666667" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.1083333333333" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19" style="3" customWidth="1"/>
-    <col min="10" max="10" width="26.225" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="21.6" customHeight="1" spans="1:10">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" ht="30" spans="1:10">
-      <c r="A2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" ht="30" spans="1:10">
-      <c r="A3" s="8"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="+32 2 551 15 72" tooltip="https://liedekerke.com/en/lawyers/tel:+3225511572"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="16.8"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More one time using it, and more fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
+++ b/src/main/resources/baseFiles/excel/RawXL/Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -36,6 +36,27 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Practice Area</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager </t>
+  </si>
+  <si>
+    <t>Specialism</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Firm</t>
   </si>
 </sst>
 </file>
@@ -1188,15 +1209,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="A2:J256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1206,6 +1227,27 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>